<commit_message>
updated report and results table
</commit_message>
<xml_diff>
--- a/results/tables/compare_gee_results.xlsx
+++ b/results/tables/compare_gee_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyz/Documents/GitHub/HEGSRR/RPr-Chakraborty-2021/results/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\hegsrr\RPr-Chakraborty-2021\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E1E42A-FD47-7D4C-8493-B02E6D979904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4B9403-E091-432A-9928-AD05D0315BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,22 +127,22 @@
     <t>&lt; 0.001</t>
   </si>
   <si>
-    <t>jay sig*</t>
-  </si>
-  <si>
     <t>* The published paper did not report p value levels more significant than 0.01</t>
   </si>
   <si>
     <t>Our Coef</t>
   </si>
   <si>
-    <t>Jay Coef</t>
-  </si>
-  <si>
     <t>Coef Diff</t>
   </si>
   <si>
     <t>QIC Diff</t>
+  </si>
+  <si>
+    <t>Orig Coef</t>
+  </si>
+  <si>
+    <t>Orig sig*</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,7 +184,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,17 +218,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,61 +515,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="8"/>
-    <col min="4" max="4" width="9.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.6640625" style="5"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" style="4"/>
+    <col min="9" max="9" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>2616.4169999999999</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>2582.5300000000002</v>
       </c>
       <c r="I3" s="4">
@@ -569,17 +578,17 @@
         <v>33.886999999999716</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>7.7229999999999999</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>7.1059999999999999</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <f>ABS(B4)-ABS(C4)</f>
         <v>0.61699999999999999</v>
       </c>
@@ -590,17 +599,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>-0.129</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
         <v>-7.400000000000001E-2</v>
       </c>
@@ -611,17 +620,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>1.9E-2</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>0.111</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>-9.1999999999999998E-2</v>
       </c>
@@ -632,17 +641,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>-3.3000000000000002E-2</v>
       </c>
@@ -653,17 +662,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>0.08</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>-5.8000000000000003E-2</v>
       </c>
@@ -674,17 +683,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>-5.5E-2</v>
       </c>
@@ -695,15 +704,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>2616.3000000000002</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>2586.5500000000002</v>
       </c>
       <c r="I10" s="4">
@@ -711,17 +720,17 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>7.7160000000000002</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>7.1859999999999999</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
         <v>0.53000000000000025</v>
       </c>
@@ -732,17 +741,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>-0.15</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>-0.23699999999999999</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <f t="shared" si="1"/>
         <v>-8.6999999999999994E-2</v>
       </c>
@@ -753,17 +762,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <v>0.11899999999999999</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <f t="shared" si="1"/>
         <v>-0.11299999999999999</v>
       </c>
@@ -774,17 +783,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>2.3E-2</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <f t="shared" si="1"/>
         <v>-9.5000000000000001E-2</v>
       </c>
@@ -795,14 +804,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>2562.674</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>2801.46</v>
       </c>
       <c r="I15" s="4">
@@ -810,17 +819,17 @@
         <v>-238.78600000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>7.774</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="6">
         <v>7.1829999999999998</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="6">
         <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
         <v>0.59100000000000019</v>
       </c>
@@ -831,17 +840,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="6">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="6">
         <f t="shared" si="2"/>
         <v>-0.13</v>
       </c>
@@ -852,17 +861,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>-0.11</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="6">
         <v>-0.26700000000000002</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="6">
         <f t="shared" si="2"/>
         <v>-0.15700000000000003</v>
       </c>
@@ -873,14 +882,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>3577.0720000000001</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>2978.7370000000001</v>
       </c>
       <c r="I19" s="4">
@@ -888,17 +897,17 @@
         <v>598.33500000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>7.7830000000000004</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="6">
         <v>7.242</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
         <v>0.54100000000000037</v>
       </c>
@@ -906,17 +915,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <v>4.7E-2</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <f t="shared" si="3"/>
         <v>-2.5000000000000001E-2</v>
       </c>
@@ -927,55 +936,55 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="6">
         <f t="shared" si="3"/>
         <v>-2.4E-2</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>-2.4E-2</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <f t="shared" si="3"/>
         <v>-1.9999999999999983E-3</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="6">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="6">
         <f t="shared" si="3"/>
         <v>-3.2999999999999995E-2</v>
       </c>
@@ -986,17 +995,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="6">
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="6">
         <v>-0.108</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="6">
         <f t="shared" si="3"/>
         <v>-5.5E-2</v>
       </c>
@@ -1007,14 +1016,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>2012.2660000000001</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>2892.35</v>
       </c>
       <c r="I26" s="4">
@@ -1022,17 +1031,17 @@
         <v>-880.08399999999983</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <v>7.7839999999999998</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <v>7.2229999999999999</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
         <v>0.56099999999999994</v>
       </c>
@@ -1043,17 +1052,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <v>-0.13500000000000001</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="6">
         <f t="shared" si="4"/>
         <v>-0.16299999999999998</v>
       </c>
@@ -1064,17 +1073,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="6">
         <v>0.153</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="6">
         <f t="shared" si="4"/>
         <v>-0.11199999999999999</v>
       </c>
@@ -1085,9 +1094,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>31</v>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement cluster based relative risk score calculation
</commit_message>
<xml_diff>
--- a/results/tables/compare_gee_results.xlsx
+++ b/results/tables/compare_gee_results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\hegsrr\RPr-Chakraborty-2021\results\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyz/Documents/GitHub/HEGSRR/RPr-Chakraborty-2021/results/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4B9403-E091-432A-9928-AD05D0315BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17103DA7-320E-6143-833B-8E52271ACAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="2600" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="37">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -88,9 +89,6 @@
     <t>female_pct</t>
   </si>
   <si>
-    <t>Table 2: GEE Equations</t>
-  </si>
-  <si>
     <t>non_hisp_white_pct</t>
   </si>
   <si>
@@ -143,6 +141,12 @@
   </si>
   <si>
     <t>Orig sig*</t>
+  </si>
+  <si>
+    <t>Table 1: GEE using local RR</t>
+  </si>
+  <si>
+    <t>Table 2: GEE using cluster RR</t>
   </si>
 </sst>
 </file>
@@ -207,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,6 +235,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,56 +522,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="A5" zoomScale="176" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" style="4"/>
-    <col min="9" max="9" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21" style="6" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.6640625" style="4"/>
+    <col min="9" max="9" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="1"/>
       <c r="G3" s="4">
@@ -578,7 +583,7 @@
         <v>33.886999999999716</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -593,13 +598,13 @@
         <v>0.61699999999999999</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,13 +619,13 @@
         <v>-7.400000000000001E-2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -635,13 +640,13 @@
         <v>-9.1999999999999998E-2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -656,13 +661,13 @@
         <v>-3.3000000000000002E-2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -677,13 +682,13 @@
         <v>-5.8000000000000003E-2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -698,15 +703,15 @@
         <v>-5.5E-2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1"/>
       <c r="G10" s="4">
@@ -720,7 +725,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,15 +740,15 @@
         <v>0.53000000000000025</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6">
         <v>-0.15</v>
@@ -756,13 +761,13 @@
         <v>-8.6999999999999994E-2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -780,10 +785,10 @@
         <v>0.19800000000000001</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -798,15 +803,15 @@
         <v>-9.5000000000000001E-2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="4">
         <v>2562.674</v>
@@ -819,7 +824,7 @@
         <v>-238.78600000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,13 +839,13 @@
         <v>0.59100000000000019</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -855,13 +860,13 @@
         <v>-0.13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -876,15 +881,15 @@
         <v>-0.15700000000000003</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19" s="4">
         <v>3577.0720000000001</v>
@@ -897,7 +902,7 @@
         <v>598.33500000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,10 +917,10 @@
         <v>0.54100000000000037</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -930,13 +935,13 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -951,11 +956,11 @@
         <v>-2.4E-2</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -970,11 +975,11 @@
         <v>-1.9999999999999983E-3</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -989,13 +994,13 @@
         <v>-3.2999999999999995E-2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1010,15 +1015,15 @@
         <v>-5.5E-2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" s="4">
         <v>2012.2660000000001</v>
@@ -1031,7 +1036,7 @@
         <v>-880.08399999999983</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,13 +1051,13 @@
         <v>0.56099999999999994</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1067,13 +1072,13 @@
         <v>-0.16299999999999998</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1088,15 +1093,15 @@
         <v>-0.11199999999999999</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1135,4 +1140,736 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFFC02A-62DD-BF4D-A4B7-E0BA8D91FFE0}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4">
+        <v>3536.585</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2582.5300000000002</v>
+      </c>
+      <c r="I3" s="4">
+        <f>G3-H3</f>
+        <v>954.05499999999984</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>7.37</v>
+      </c>
+      <c r="C4" s="6">
+        <v>7.1059999999999999</v>
+      </c>
+      <c r="D4" s="6">
+        <f>ABS(B4)-ABS(C4)</f>
+        <v>0.26400000000000023</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
+        <v>-4.0000000000000008E-2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.104</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.111</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.0000000000000062E-3</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="C7" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4">
+        <v>3551.125</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2586.5500000000002</v>
+      </c>
+      <c r="I10" s="4">
+        <f>G10-H10</f>
+        <v>964.57499999999982</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6">
+        <v>7.36</v>
+      </c>
+      <c r="C11" s="6">
+        <v>7.1859999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
+        <v>0.17400000000000038</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6">
+        <v>-0.19</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-0.23699999999999999</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="1"/>
+        <v>-4.6999999999999986E-2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.11399999999999999</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="1"/>
+        <v>-1.2999999999999998E-2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="4">
+        <v>3661.1990000000001</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2801.46</v>
+      </c>
+      <c r="I15" s="4">
+        <f>G15-H15</f>
+        <v>859.73900000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6">
+        <v>7.3819999999999997</v>
+      </c>
+      <c r="C16" s="6">
+        <v>7.1829999999999998</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
+        <v>0.19899999999999984</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.109</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="2"/>
+        <v>-3.8999999999999993E-2</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-0.19400000000000001</v>
+      </c>
+      <c r="C18" s="6">
+        <v>-0.26700000000000002</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>-7.3000000000000009E-2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="4">
+        <v>3570.62</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2978.7370000000001</v>
+      </c>
+      <c r="I19" s="4">
+        <f>G19-H19</f>
+        <v>591.88299999999981</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7.4219999999999997</v>
+      </c>
+      <c r="C20" s="6">
+        <v>7.242</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
+        <v>0.17999999999999972</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.9E-2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="6">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1999999999999999E-2</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="6">
+        <v>-7.2999999999999995E-2</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6E-2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="6">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-0.108</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="3"/>
+        <v>-2.8999999999999998E-2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="4">
+        <v>3534.64</v>
+      </c>
+      <c r="H26" s="4">
+        <v>2892.35</v>
+      </c>
+      <c r="I26" s="4">
+        <f>G26-H26</f>
+        <v>642.29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="6">
+        <v>7.4210000000000003</v>
+      </c>
+      <c r="C27" s="6">
+        <v>7.2229999999999999</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
+        <v>0.1980000000000004</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6">
+        <v>-0.222</v>
+      </c>
+      <c r="C28" s="6">
+        <v>-0.29799999999999999</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="4"/>
+        <v>-7.5999999999999984E-2</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0.121</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.153</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="4"/>
+        <v>-3.2000000000000001E-2</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D31">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5B23843F-3191-144B-9978-0CA7C943994D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5B23843F-3191-144B-9978-0CA7C943994D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D31</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new blank gee sheet
</commit_message>
<xml_diff>
--- a/results/tables/compare_gee_results.xlsx
+++ b/results/tables/compare_gee_results.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2595" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="4260" yWindow="2595" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="LocalRR" sheetId="1" r:id="rId1"/>
-    <sheet name="ClusterRR" sheetId="2" r:id="rId2"/>
+    <sheet name="OriginalData" sheetId="4" r:id="rId1"/>
+    <sheet name="LocalRR" sheetId="1" r:id="rId2"/>
+    <sheet name="ClusterRR" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="38">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -524,6 +525,644 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4">
+        <v>3536.585</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2582.5300000000002</v>
+      </c>
+      <c r="I3" s="4">
+        <f>G3-H3</f>
+        <v>954.05499999999984</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6">
+        <v>7.1059999999999999</v>
+      </c>
+      <c r="D4" s="6">
+        <f>ABS(B4)-ABS(C4)</f>
+        <v>-7.1059999999999999</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6">
+        <v>0.111</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.111</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>-5.0999999999999997E-2</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.08</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>-7.6999999999999999E-2</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
+        <v>2586.5500000000002</v>
+      </c>
+      <c r="I10" s="4">
+        <f>G10-H10</f>
+        <v>-2586.5500000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6">
+        <v>7.1859999999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
+        <v>-7.1859999999999999</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6">
+        <v>-0.23699999999999999</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.23699999999999999</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.11899999999999999</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.11799999999999999</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
+        <v>2801.46</v>
+      </c>
+      <c r="I15" s="4">
+        <f>G15-H15</f>
+        <v>-2801.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6">
+        <v>7.1829999999999998</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
+        <v>-7.1829999999999998</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.14799999999999999</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6">
+        <v>-0.26700000000000002</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="2"/>
+        <v>-0.26700000000000002</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>2978.7370000000001</v>
+      </c>
+      <c r="I19" s="4">
+        <f>G19-H19</f>
+        <v>-2978.7370000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6">
+        <v>7.242</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
+        <v>-7.242</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="3"/>
+        <v>-4.7E-2</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" si="3"/>
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" si="3"/>
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="3"/>
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6">
+        <v>-0.108</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.108</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4">
+        <v>2892.35</v>
+      </c>
+      <c r="I26" s="4">
+        <f>G26-H26</f>
+        <v>-2892.35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6">
+        <v>7.2229999999999999</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
+        <v>-7.2229999999999999</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6">
+        <v>-0.29799999999999999</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="4"/>
+        <v>-0.29799999999999999</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6">
+        <v>0.153</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" si="4"/>
+        <v>-0.153</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D31">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C9D9A169-582F-433C-AAF8-4A77F5D26ED8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C9D9A169-582F-433C-AAF8-4A77F5D26ED8}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D31</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,11 +1783,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update compare_gee using original data
</commit_message>
<xml_diff>
--- a/results/tables/compare_gee_results.xlsx
+++ b/results/tables/compare_gee_results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josephh\Documents\GitHub\hegsrr\RPr-Chakraborty2020\results\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyz/Documents/GitHub/HEGSRR/RPr-Chakraborty-2021/results/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545CD843-E33E-204E-A348-DEE7081F328D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2595" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="560" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="OriginalData" sheetId="4" r:id="rId1"/>
+    <sheet name="OriginalData" sheetId="5" r:id="rId1"/>
     <sheet name="LocalRR" sheetId="1" r:id="rId2"/>
     <sheet name="ClusterRR" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="38">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -155,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -522,22 +523,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBFDB80-550D-E547-8762-E7B90E35A6B3}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G26"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -547,7 +550,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>30</v>
@@ -574,7 +577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -584,29 +587,33 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4">
-        <v>3536.585</v>
+        <v>6181.4120000000003</v>
       </c>
       <c r="H3" s="4">
         <v>2582.5300000000002</v>
       </c>
       <c r="I3" s="4">
         <f>G3-H3</f>
-        <v>954.05499999999984</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3598.8820000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>6.7809999999999997</v>
+      </c>
       <c r="C4" s="6">
         <v>7.1059999999999999</v>
       </c>
       <c r="D4" s="6">
         <f>ABS(B4)-ABS(C4)</f>
-        <v>-7.1059999999999999</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>-0.32500000000000018</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
@@ -614,19 +621,23 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <v>-0.20300000000000001</v>
+      </c>
       <c r="C5" s="6">
         <v>-0.20300000000000001</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
-        <v>-0.20300000000000001</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
@@ -634,19 +645,23 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <v>0.33900000000000002</v>
+      </c>
       <c r="C6" s="6">
         <v>0.111</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>-0.111</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>0.22800000000000004</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="F6" s="9" t="s">
         <v>26</v>
       </c>
@@ -654,39 +669,47 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <v>0.02</v>
+      </c>
       <c r="C7" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>-5.0999999999999997E-2</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
+        <v>-3.0999999999999996E-2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6">
+        <v>5.8000000000000003E-2</v>
+      </c>
       <c r="C8" s="6">
         <v>0.08</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>-0.08</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
@@ -694,27 +717,31 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <v>0.108</v>
+      </c>
       <c r="C9" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>-7.6999999999999999E-2</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -723,28 +750,34 @@
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4">
+        <v>6176.2079999999996</v>
+      </c>
       <c r="H10" s="4">
         <v>2586.5500000000002</v>
       </c>
       <c r="I10" s="4">
         <f>G10-H10</f>
-        <v>-2586.5500000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3589.6579999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <v>6.7720000000000002</v>
+      </c>
       <c r="C11" s="6">
         <v>7.1859999999999999</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
-        <v>-7.1859999999999999</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>-0.4139999999999997</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>26</v>
       </c>
@@ -752,19 +785,23 @@
       <c r="H11" s="4"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6">
+        <v>-0.22800000000000001</v>
+      </c>
       <c r="C12" s="6">
         <v>-0.23699999999999999</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="1"/>
-        <v>-0.23699999999999999</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>-8.9999999999999802E-3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>26</v>
       </c>
@@ -772,39 +809,47 @@
       <c r="H12" s="4"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6">
+        <v>0.13200000000000001</v>
+      </c>
       <c r="C13" s="6">
         <v>0.11899999999999999</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="1"/>
-        <v>-0.11899999999999999</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6">
+        <v>0.33500000000000002</v>
+      </c>
       <c r="C14" s="6">
         <v>0.11799999999999999</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="1"/>
-        <v>-0.11799999999999999</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>0.21700000000000003</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
@@ -812,7 +857,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -820,28 +865,34 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4">
+        <v>6171.74</v>
+      </c>
       <c r="H15" s="4">
         <v>2801.46</v>
       </c>
       <c r="I15" s="4">
         <f>G15-H15</f>
-        <v>-2801.46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3370.2799999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6">
+        <v>6.8490000000000002</v>
+      </c>
       <c r="C16" s="6">
         <v>7.1829999999999998</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
-        <v>-7.1829999999999998</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>-0.33399999999999963</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>26</v>
       </c>
@@ -849,19 +900,23 @@
       <c r="H16" s="4"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6">
+        <v>0.28299999999999997</v>
+      </c>
       <c r="C17" s="6">
         <v>0.14799999999999999</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="2"/>
-        <v>-0.14799999999999999</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>26</v>
       </c>
@@ -869,19 +924,23 @@
       <c r="H17" s="4"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="6">
+        <v>-0.315</v>
+      </c>
       <c r="C18" s="6">
         <v>-0.26700000000000002</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="2"/>
-        <v>-0.26700000000000002</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>4.7999999999999987E-2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>26</v>
       </c>
@@ -889,7 +948,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -897,28 +956,34 @@
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4">
+        <v>6180.9669999999996</v>
+      </c>
       <c r="H19" s="4">
         <v>2978.7370000000001</v>
       </c>
       <c r="I19" s="4">
         <f>G19-H19</f>
-        <v>-2978.7370000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3202.2299999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="6">
+        <v>6.8639999999999999</v>
+      </c>
       <c r="C20" s="6">
         <v>7.242</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
-        <v>-7.242</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>-0.37800000000000011</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>26</v>
       </c>
@@ -926,19 +991,23 @@
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="6">
+        <v>7.6999999999999999E-2</v>
+      </c>
       <c r="C21" s="6">
         <v>4.7E-2</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="3"/>
-        <v>-4.7E-2</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>26</v>
       </c>
@@ -946,75 +1015,91 @@
       <c r="H21" s="4"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="C22" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="3"/>
-        <v>-3.7999999999999999E-2</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+        <v>-1.2E-2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="6">
+        <v>0.04</v>
+      </c>
       <c r="C23" s="6">
         <v>-2.5999999999999999E-2</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="3"/>
-        <v>-2.5999999999999999E-2</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+        <v>1.4000000000000002E-2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="F23" s="7"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="6">
+        <v>-2.4E-2</v>
+      </c>
       <c r="C24" s="6">
         <v>-8.8999999999999996E-2</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="3"/>
-        <v>-8.8999999999999996E-2</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
+        <v>-6.5000000000000002E-2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6">
+        <v>-0.2</v>
+      </c>
       <c r="C25" s="6">
         <v>-0.108</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="3"/>
-        <v>-0.108</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>9.2000000000000012E-2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1022,7 +1107,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1030,28 +1115,34 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4">
+        <v>6173.25</v>
+      </c>
       <c r="H26" s="4">
         <v>2892.35</v>
       </c>
       <c r="I26" s="4">
         <f>G26-H26</f>
-        <v>-2892.35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3280.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="6">
+        <v>6.85</v>
+      </c>
       <c r="C27" s="6">
         <v>7.2229999999999999</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
-        <v>-7.2229999999999999</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>-0.37300000000000022</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1059,19 +1150,23 @@
       <c r="H27" s="4"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="6">
+        <v>-0.46700000000000003</v>
+      </c>
       <c r="C28" s="6">
         <v>-0.29799999999999999</v>
       </c>
       <c r="D28" s="6">
         <f t="shared" si="4"/>
-        <v>-0.29799999999999999</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>0.16900000000000004</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1079,52 +1174,32 @@
       <c r="H28" s="4"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="6">
+        <v>0.38</v>
+      </c>
       <c r="C29" s="6">
         <v>0.153</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" si="4"/>
-        <v>-0.153</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="H29" s="4"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D31">
+  <conditionalFormatting sqref="D1:D29">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1133,7 +1208,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{C9D9A169-582F-433C-AAF8-4A77F5D26ED8}</x14:id>
+          <x14:id>{5813707B-5655-9542-8634-B28E191F8129}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1143,7 +1218,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C9D9A169-582F-433C-AAF8-4A77F5D26ED8}">
+          <x14:cfRule type="dataBar" id="{5813707B-5655-9542-8634-B28E191F8129}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -1151,7 +1226,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D1:D31</xm:sqref>
+          <xm:sqref>D1:D29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1160,29 +1235,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="21" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" style="4"/>
-    <col min="9" max="9" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.6640625" style="4"/>
+    <col min="9" max="9" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
@@ -1208,7 +1285,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1224,7 +1301,7 @@
         <v>33.886999999999716</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1266,7 +1343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1308,7 +1385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1329,7 +1406,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1350,7 +1427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1366,7 +1443,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1408,7 +1485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1429,7 +1506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1450,7 +1527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1465,7 +1542,7 @@
         <v>-238.78600000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1563,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1507,7 +1584,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1528,7 +1605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1543,7 +1620,7 @@
         <v>598.33500000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1561,7 +1638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1582,7 +1659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1601,7 +1678,7 @@
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1620,7 +1697,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1641,7 +1718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1662,7 +1739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1677,7 +1754,7 @@
         <v>-880.08399999999983</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1698,7 +1775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1719,7 +1796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1740,7 +1817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -1784,20 +1861,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -1809,7 +1886,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>30</v>
@@ -1836,7 +1913,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1856,7 +1933,7 @@
         <v>954.05499999999984</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1880,7 +1957,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1904,7 +1981,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1928,7 +2005,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1952,7 +2029,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1976,7 +2053,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2000,7 +2077,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2020,7 +2097,7 @@
         <v>964.57499999999982</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2121,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -2068,7 +2145,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2092,7 +2169,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2116,7 +2193,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2135,7 +2212,7 @@
         <v>859.73900000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2236,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -2183,7 +2260,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -2207,7 +2284,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -2226,7 +2303,7 @@
         <v>591.88299999999981</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2327,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -2274,7 +2351,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2296,7 +2373,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2318,7 +2395,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2342,7 +2419,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2366,7 +2443,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2385,7 +2462,7 @@
         <v>642.29</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2409,7 +2486,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -2433,7 +2510,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -2459,7 +2536,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -2469,7 +2546,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
updated table with final comparison
</commit_message>
<xml_diff>
--- a/results/tables/compare_gee_results.xlsx
+++ b/results/tables/compare_gee_results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyz/Documents/GitHub/HEGSRR/RPr-Chakraborty-2021/results/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josephh\Documents\GitHub\hegsrr\RPr-Chakraborty2020\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545CD843-E33E-204E-A348-DEE7081F328D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="560" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="555" windowWidth="28800" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OriginalData" sheetId="5" r:id="rId1"/>
     <sheet name="LocalRR" sheetId="1" r:id="rId2"/>
     <sheet name="ClusterRR" sheetId="2" r:id="rId3"/>
+    <sheet name="CompareCoefficients" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="44">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -151,14 +151,33 @@
   </si>
   <si>
     <t>ew</t>
+  </si>
+  <si>
+    <t>Table 1: GEE using author's data</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Original Publication</t>
+  </si>
+  <si>
+    <t>Reproduce with Author's Data in R</t>
+  </si>
+  <si>
+    <t>Reanalyze with Local RR in R</t>
+  </si>
+  <si>
+    <t>Reanalyze with Cluster RR in R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -215,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +261,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -523,24 +557,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBFDB80-550D-E547-8762-E7B90E35A6B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -550,7 +584,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>30</v>
@@ -577,7 +611,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -597,7 +631,7 @@
         <v>3598.8820000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -621,7 +655,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -645,7 +679,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -669,7 +703,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -693,7 +727,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -717,7 +751,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -741,7 +775,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -761,7 +795,7 @@
         <v>3589.6579999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +819,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -809,7 +843,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -833,7 +867,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -857,7 +891,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -876,7 +910,7 @@
         <v>3370.2799999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +934,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -924,7 +958,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -948,7 +982,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -967,7 +1001,7 @@
         <v>3202.2299999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1025,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1049,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1071,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1059,7 +1093,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1083,7 +1117,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1107,7 +1141,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1126,7 +1160,7 @@
         <v>3280.9</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1184,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1174,7 +1208,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1235,31 +1269,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B4" sqref="B4:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="21" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.6640625" style="4"/>
-    <col min="9" max="9" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" style="4"/>
+    <col min="9" max="9" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
@@ -1285,7 +1319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1301,7 +1335,7 @@
         <v>33.886999999999716</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1322,7 +1356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1343,7 +1377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1385,7 +1419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1406,7 +1440,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1427,7 +1461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1443,7 +1477,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1464,7 +1498,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1519,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1506,7 +1540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1542,7 +1576,7 @@
         <v>-238.78600000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1563,7 +1597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1584,7 +1618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1605,7 +1639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1620,7 +1654,7 @@
         <v>598.33500000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1672,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1659,7 +1693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1678,7 +1712,7 @@
       </c>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1697,7 +1731,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1718,7 +1752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1739,7 +1773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1754,7 +1788,7 @@
         <v>-880.08399999999983</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1796,7 +1830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1817,7 +1851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -1861,20 +1895,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -1886,7 +1920,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>30</v>
@@ -1913,7 +1947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1933,7 +1967,7 @@
         <v>954.05499999999984</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1957,7 +1991,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1981,7 +2015,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2005,7 +2039,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2029,7 +2063,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2087,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -2077,7 +2111,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -2097,7 +2131,7 @@
         <v>964.57499999999982</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2155,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -2145,7 +2179,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2169,7 +2203,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -2193,7 +2227,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2212,7 +2246,7 @@
         <v>859.73900000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2270,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -2260,7 +2294,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -2284,7 +2318,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -2303,7 +2337,7 @@
         <v>591.88299999999981</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2327,7 +2361,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
@@ -2351,7 +2385,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -2373,7 +2407,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2395,7 +2429,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2419,7 +2453,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2443,7 +2477,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2462,7 +2496,7 @@
         <v>642.29</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2486,7 +2520,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -2510,7 +2544,7 @@
       <c r="H28" s="4"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -2536,7 +2570,7 @@
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -2546,7 +2580,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -2592,4 +2626,549 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6">
+        <v>7.1059999999999999</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6.7809999999999997</v>
+      </c>
+      <c r="D3" s="6">
+        <v>7.7229999999999999</v>
+      </c>
+      <c r="E3" s="6">
+        <v>7.37</v>
+      </c>
+      <c r="F3" s="14">
+        <f>_xlfn.VAR.P(B3:E3)</f>
+        <v>0.11968150000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-0.20300000000000001</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-0.129</v>
+      </c>
+      <c r="E4" s="6">
+        <v>-0.16300000000000001</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:F8" si="0">_xlfn.VAR.P(B4:E4)</f>
+        <v>9.5674999999999927E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.111</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.104</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="0"/>
+        <v>1.4084187499999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="0"/>
+        <v>1.7868750000000003E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="C7" s="6">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>4.6718749999999972E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.108</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="0"/>
+        <v>1.6011874999999989E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6">
+        <v>7.1859999999999999</v>
+      </c>
+      <c r="C10" s="6">
+        <v>6.7720000000000002</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7.7160000000000002</v>
+      </c>
+      <c r="E10" s="6">
+        <v>7.36</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" ref="F10:F28" si="1">_xlfn.VAR.P(B10:E10)</f>
+        <v>0.11538675</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6">
+        <v>-0.23699999999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-0.22800000000000001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-0.15</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-0.19</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="1"/>
+        <v>1.1866875000000054E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D12" s="6">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="1"/>
+        <v>3.6212499999999995E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="1"/>
+        <v>1.3328187499999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6">
+        <v>7.1829999999999998</v>
+      </c>
+      <c r="C15" s="6">
+        <v>6.8490000000000002</v>
+      </c>
+      <c r="D15" s="6">
+        <v>7.774</v>
+      </c>
+      <c r="E15" s="6">
+        <v>7.3819999999999997</v>
+      </c>
+      <c r="F15" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11211349999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.109</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="1"/>
+        <v>9.0892500000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6">
+        <v>-0.26700000000000002</v>
+      </c>
+      <c r="C17" s="6">
+        <v>-0.315</v>
+      </c>
+      <c r="D17" s="6">
+        <v>-0.11</v>
+      </c>
+      <c r="E17" s="6">
+        <v>-0.19400000000000001</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" si="1"/>
+        <v>6.0002499999999848E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.242</v>
+      </c>
+      <c r="C19" s="6">
+        <v>6.8639999999999999</v>
+      </c>
+      <c r="D19" s="6">
+        <v>7.7830000000000004</v>
+      </c>
+      <c r="E19" s="6">
+        <v>7.4219999999999997</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="1"/>
+        <v>0.10963818750000009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="6">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C20" s="6">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F20" s="14">
+        <f t="shared" si="1"/>
+        <v>4.5925000000000002E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F21" s="14">
+        <f t="shared" si="1"/>
+        <v>1.6274999999999992E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="6">
+        <v>-2.5999999999999999E-2</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="D22" s="6">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="E22" s="6">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="F22" s="14">
+        <f t="shared" si="1"/>
+        <v>7.2600000000000008E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="6">
+        <v>-8.8999999999999996E-2</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="D23" s="6">
+        <v>-5.6000000000000001E-2</v>
+      </c>
+      <c r="E23" s="6">
+        <v>-7.2999999999999995E-2</v>
+      </c>
+      <c r="F23" s="14">
+        <f t="shared" si="1"/>
+        <v>5.802499999999996E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="6">
+        <v>-0.108</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-0.2</v>
+      </c>
+      <c r="D24" s="6">
+        <v>-5.2999999999999999E-2</v>
+      </c>
+      <c r="E24" s="6">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+      <c r="F24" s="14">
+        <f t="shared" si="1"/>
+        <v>3.0785000000000014E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="6">
+        <v>7.2229999999999999</v>
+      </c>
+      <c r="C26" s="6">
+        <v>6.85</v>
+      </c>
+      <c r="D26" s="6">
+        <v>7.7839999999999998</v>
+      </c>
+      <c r="E26" s="6">
+        <v>7.4210000000000003</v>
+      </c>
+      <c r="F26" s="14">
+        <f t="shared" si="1"/>
+        <v>0.11395125000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="6">
+        <v>-0.29799999999999999</v>
+      </c>
+      <c r="C27" s="6">
+        <v>-0.46700000000000003</v>
+      </c>
+      <c r="D27" s="6">
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="E27" s="6">
+        <v>-0.222</v>
+      </c>
+      <c r="F27" s="14">
+        <f t="shared" si="1"/>
+        <v>1.4920249999999982E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0.153</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="D28" s="6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.121</v>
+      </c>
+      <c r="F28" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5843687499999985E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added tables to the results to compare the computational environments
</commit_message>
<xml_diff>
--- a/results/tables/compare_gee_results.xlsx
+++ b/results/tables/compare_gee_results.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="555" windowWidth="28800" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="555" windowWidth="28800" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OriginalData" sheetId="5" r:id="rId1"/>
     <sheet name="LocalRR" sheetId="1" r:id="rId2"/>
     <sheet name="ClusterRR" sheetId="2" r:id="rId3"/>
     <sheet name="CompareCoefficients" sheetId="6" r:id="rId4"/>
+    <sheet name="ComareAverageCoefficients" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" iterate="1"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="56">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -150,9 +151,6 @@
     <t>Table 2: GEE using cluster RR</t>
   </si>
   <si>
-    <t>ew</t>
-  </si>
-  <si>
     <t>Table 1: GEE using author's data</t>
   </si>
   <si>
@@ -169,6 +167,45 @@
   </si>
   <si>
     <t>Reanalyze with Cluster RR in R</t>
+  </si>
+  <si>
+    <t>Diff to Original</t>
+  </si>
+  <si>
+    <t>Diff to Orig in R</t>
+  </si>
+  <si>
+    <t>Average Difference</t>
+  </si>
+  <si>
+    <t>Original Study</t>
+  </si>
+  <si>
+    <t>Original Data in R/geepack</t>
+  </si>
+  <si>
+    <t>Reproduced local relative risk</t>
+  </si>
+  <si>
+    <t>Reproduced cluster relative risk</t>
+  </si>
+  <si>
+    <t>Diff to Local RR</t>
+  </si>
+  <si>
+    <t>H2.1 Race Model</t>
+  </si>
+  <si>
+    <t>H2.2 Ethnicity Model</t>
+  </si>
+  <si>
+    <t>H2.3 Poverty Model</t>
+  </si>
+  <si>
+    <t>H2.4 Age Model</t>
+  </si>
+  <si>
+    <t>H2.5 Biological Sex Model</t>
   </si>
 </sst>
 </file>
@@ -179,7 +216,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +234,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,6 +323,24 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,23 +621,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B29"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -638,10 +701,10 @@
       <c r="B4" s="6">
         <v>6.7809999999999997</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="14">
         <v>7.1059999999999999</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="14">
         <f>ABS(B4)-ABS(C4)</f>
         <v>-0.32500000000000018</v>
       </c>
@@ -662,10 +725,10 @@
       <c r="B5" s="6">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="14">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="14">
         <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
         <v>0</v>
       </c>
@@ -686,10 +749,10 @@
       <c r="B6" s="6">
         <v>0.33900000000000002</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="14">
         <v>0.111</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>0.22800000000000004</v>
       </c>
@@ -710,10 +773,10 @@
       <c r="B7" s="6">
         <v>0.02</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="14">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="14">
         <f t="shared" si="0"/>
         <v>-3.0999999999999996E-2</v>
       </c>
@@ -734,10 +797,10 @@
       <c r="B8" s="6">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="14">
         <v>0.08</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>-2.1999999999999999E-2</v>
       </c>
@@ -758,10 +821,10 @@
       <c r="B9" s="6">
         <v>0.108</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="14">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>3.1E-2</v>
       </c>
@@ -780,8 +843,8 @@
         <v>22</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="4">
@@ -802,10 +865,10 @@
       <c r="B11" s="6">
         <v>6.7720000000000002</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="14">
         <v>7.1859999999999999</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="14">
         <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
         <v>-0.4139999999999997</v>
       </c>
@@ -826,10 +889,10 @@
       <c r="B12" s="6">
         <v>-0.22800000000000001</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="14">
         <v>-0.23699999999999999</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="14">
         <f t="shared" si="1"/>
         <v>-8.9999999999999802E-3</v>
       </c>
@@ -850,10 +913,10 @@
       <c r="B13" s="6">
         <v>0.13200000000000001</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="14">
         <v>0.11899999999999999</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="14">
         <f t="shared" si="1"/>
         <v>1.3000000000000012E-2</v>
       </c>
@@ -874,10 +937,10 @@
       <c r="B14" s="6">
         <v>0.33500000000000002</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="14">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="14">
         <f t="shared" si="1"/>
         <v>0.21700000000000003</v>
       </c>
@@ -896,8 +959,8 @@
         <v>23</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="F15" s="1"/>
       <c r="G15" s="4">
         <v>6171.74</v>
@@ -917,10 +980,10 @@
       <c r="B16" s="6">
         <v>6.8490000000000002</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="14">
         <v>7.1829999999999998</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="14">
         <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
         <v>-0.33399999999999963</v>
       </c>
@@ -941,10 +1004,10 @@
       <c r="B17" s="6">
         <v>0.28299999999999997</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="14">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="14">
         <f t="shared" si="2"/>
         <v>0.13499999999999998</v>
       </c>
@@ -965,10 +1028,10 @@
       <c r="B18" s="6">
         <v>-0.315</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="14">
         <v>-0.26700000000000002</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="14">
         <f t="shared" si="2"/>
         <v>4.7999999999999987E-2</v>
       </c>
@@ -987,8 +1050,8 @@
         <v>24</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
       <c r="F19" s="1"/>
       <c r="G19" s="4">
         <v>6180.9669999999996</v>
@@ -1008,10 +1071,10 @@
       <c r="B20" s="6">
         <v>6.8639999999999999</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="14">
         <v>7.242</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="14">
         <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
         <v>-0.37800000000000011</v>
       </c>
@@ -1032,10 +1095,10 @@
       <c r="B21" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="14">
         <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
@@ -1056,10 +1119,10 @@
       <c r="B22" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="14">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="14">
         <f t="shared" si="3"/>
         <v>-1.2E-2</v>
       </c>
@@ -1078,10 +1141,10 @@
       <c r="B23" s="6">
         <v>0.04</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="14">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="14">
         <f t="shared" si="3"/>
         <v>1.4000000000000002E-2</v>
       </c>
@@ -1100,10 +1163,10 @@
       <c r="B24" s="6">
         <v>-2.4E-2</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="14">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="14">
         <f t="shared" si="3"/>
         <v>-6.5000000000000002E-2</v>
       </c>
@@ -1124,10 +1187,10 @@
       <c r="B25" s="6">
         <v>-0.2</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="14">
         <v>-0.108</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="14">
         <f t="shared" si="3"/>
         <v>9.2000000000000012E-2</v>
       </c>
@@ -1146,8 +1209,8 @@
         <v>25</v>
       </c>
       <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
       <c r="F26" s="1"/>
       <c r="G26" s="4">
         <v>6173.25</v>
@@ -1167,10 +1230,10 @@
       <c r="B27" s="6">
         <v>6.85</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="14">
         <v>7.2229999999999999</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="14">
         <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
         <v>-0.37300000000000022</v>
       </c>
@@ -1191,10 +1254,10 @@
       <c r="B28" s="6">
         <v>-0.46700000000000003</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="14">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="14">
         <f t="shared" si="4"/>
         <v>0.16900000000000004</v>
       </c>
@@ -1215,10 +1278,10 @@
       <c r="B29" s="6">
         <v>0.38</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="14">
         <v>0.153</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="14">
         <f t="shared" si="4"/>
         <v>0.22700000000000001</v>
       </c>
@@ -1231,6 +1294,9 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D29">
@@ -1273,15 +1339,15 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B29"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="21" style="14" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.7109375" style="4"/>
@@ -1294,13 +1360,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1339,13 +1405,13 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="14">
         <v>7.7229999999999999</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="14">
         <v>7.1059999999999999</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="14">
         <f>ABS(B4)-ABS(C4)</f>
         <v>0.61699999999999999</v>
       </c>
@@ -1360,13 +1426,13 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="14">
         <v>-0.129</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="14">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="14">
         <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
         <v>-7.400000000000001E-2</v>
       </c>
@@ -1381,13 +1447,13 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="14">
         <v>1.9E-2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="14">
         <v>0.111</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>-9.1999999999999998E-2</v>
       </c>
@@ -1402,13 +1468,13 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="14">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="14">
         <f t="shared" si="0"/>
         <v>-3.3000000000000002E-2</v>
       </c>
@@ -1423,13 +1489,13 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="14">
         <v>0.08</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>-5.8000000000000003E-2</v>
       </c>
@@ -1444,13 +1510,13 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="14">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>-5.5E-2</v>
       </c>
@@ -1481,13 +1547,13 @@
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="14">
         <v>7.7160000000000002</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="14">
         <v>7.1859999999999999</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="14">
         <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
         <v>0.53000000000000025</v>
       </c>
@@ -1502,13 +1568,13 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="14">
         <v>-0.15</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="14">
         <v>-0.23699999999999999</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="14">
         <f t="shared" si="1"/>
         <v>-8.6999999999999994E-2</v>
       </c>
@@ -1523,13 +1589,13 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="14">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="14">
         <v>0.11899999999999999</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="14">
         <f t="shared" si="1"/>
         <v>-0.11299999999999999</v>
       </c>
@@ -1544,13 +1610,13 @@
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="14">
         <v>2.3E-2</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="14">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="14">
         <f t="shared" si="1"/>
         <v>-9.5000000000000001E-2</v>
       </c>
@@ -1580,13 +1646,13 @@
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="14">
         <v>7.774</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="14">
         <v>7.1829999999999998</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="14">
         <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
         <v>0.59100000000000019</v>
       </c>
@@ -1601,13 +1667,13 @@
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="14">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="14">
         <f t="shared" si="2"/>
         <v>-0.13</v>
       </c>
@@ -1622,13 +1688,13 @@
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="14">
         <v>-0.11</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="14">
         <v>-0.26700000000000002</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="14">
         <f t="shared" si="2"/>
         <v>-0.15700000000000003</v>
       </c>
@@ -1658,13 +1724,13 @@
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="14">
         <v>7.7830000000000004</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="14">
         <v>7.242</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="14">
         <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
         <v>0.54100000000000037</v>
       </c>
@@ -1676,13 +1742,13 @@
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="14">
         <f t="shared" si="3"/>
         <v>-2.5000000000000001E-2</v>
       </c>
@@ -1697,13 +1763,13 @@
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="14">
         <v>1.4E-2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="14">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="14">
         <f t="shared" si="3"/>
         <v>-2.4E-2</v>
       </c>
@@ -1716,13 +1782,13 @@
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="14">
         <v>-2.4E-2</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="14">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="14">
         <f t="shared" si="3"/>
         <v>-1.9999999999999983E-3</v>
       </c>
@@ -1735,13 +1801,13 @@
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="14">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="14">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="14">
         <f t="shared" si="3"/>
         <v>-3.2999999999999995E-2</v>
       </c>
@@ -1756,13 +1822,13 @@
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="14">
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="14">
         <v>-0.108</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="14">
         <f t="shared" si="3"/>
         <v>-5.5E-2</v>
       </c>
@@ -1792,13 +1858,13 @@
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="14">
         <v>7.7839999999999998</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="14">
         <v>7.2229999999999999</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="14">
         <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
         <v>0.56099999999999994</v>
       </c>
@@ -1813,13 +1879,13 @@
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="14">
         <v>-0.13500000000000001</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="14">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="14">
         <f t="shared" si="4"/>
         <v>-0.16299999999999998</v>
       </c>
@@ -1834,13 +1900,13 @@
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="14">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="14">
         <v>0.153</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="14">
         <f t="shared" si="4"/>
         <v>-0.11199999999999999</v>
       </c>
@@ -1854,6 +1920,10 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="I31" s="4">
+        <f>AVERAGE(I3:I28)</f>
+        <v>-91.379600000000025</v>
       </c>
     </row>
   </sheetData>
@@ -1898,23 +1968,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="17"/>
+    <col min="4" max="4" width="19.28515625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
       <c r="F1" s="1"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -1922,13 +1993,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1951,9 +2022,9 @@
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4">
@@ -1971,13 +2042,13 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="14">
         <v>7.37</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="14">
         <v>7.1059999999999999</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="14">
         <f>ABS(B4)-ABS(C4)</f>
         <v>0.26400000000000023</v>
       </c>
@@ -1995,13 +2066,13 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="14">
         <v>-0.16300000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="14">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="14">
         <f t="shared" ref="D5:D9" si="0">ABS(B5)-ABS(C5)</f>
         <v>-4.0000000000000008E-2</v>
       </c>
@@ -2019,13 +2090,13 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="14">
         <v>0.104</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="14">
         <v>0.111</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>-7.0000000000000062E-3</v>
       </c>
@@ -2043,13 +2114,13 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="14">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="14">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="14">
         <f t="shared" si="0"/>
         <v>-1.4999999999999999E-2</v>
       </c>
@@ -2067,13 +2138,13 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="14">
         <v>3.9E-2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="14">
         <v>0.08</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="14">
         <f t="shared" si="0"/>
         <v>-4.1000000000000002E-2</v>
       </c>
@@ -2091,13 +2162,13 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="14">
         <v>0.01</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="14">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="14">
         <f t="shared" si="0"/>
         <v>-6.7000000000000004E-2</v>
       </c>
@@ -2115,9 +2186,9 @@
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="4">
@@ -2135,13 +2206,13 @@
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="14">
         <v>7.36</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="14">
         <v>7.1859999999999999</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="14">
         <f t="shared" ref="D11:D14" si="1">ABS(B11)-ABS(C11)</f>
         <v>0.17400000000000038</v>
       </c>
@@ -2159,13 +2230,13 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="14">
         <v>-0.19</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="14">
         <v>-0.23699999999999999</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="14">
         <f t="shared" si="1"/>
         <v>-4.6999999999999986E-2</v>
       </c>
@@ -2183,13 +2254,13 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="14">
         <v>0.11899999999999999</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="14">
         <f t="shared" si="1"/>
         <v>-0.11399999999999999</v>
       </c>
@@ -2207,13 +2278,13 @@
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="14">
         <v>0.105</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="14">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="14">
         <f t="shared" si="1"/>
         <v>-1.2999999999999998E-2</v>
       </c>
@@ -2231,9 +2302,9 @@
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="F15" s="1"/>
       <c r="G15" s="4">
         <v>3661.1990000000001</v>
@@ -2250,13 +2321,13 @@
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="14">
         <v>7.3819999999999997</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="14">
         <v>7.1829999999999998</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="14">
         <f t="shared" ref="D16:D18" si="2">ABS(B16)-ABS(C16)</f>
         <v>0.19899999999999984</v>
       </c>
@@ -2274,13 +2345,13 @@
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="14">
         <v>0.109</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="14">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="14">
         <f t="shared" si="2"/>
         <v>-3.8999999999999993E-2</v>
       </c>
@@ -2298,13 +2369,13 @@
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="14">
         <v>-0.19400000000000001</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="14">
         <v>-0.26700000000000002</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="14">
         <f t="shared" si="2"/>
         <v>-7.3000000000000009E-2</v>
       </c>
@@ -2322,9 +2393,9 @@
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
       <c r="F19" s="1"/>
       <c r="G19" s="4">
         <v>3570.62</v>
@@ -2341,13 +2412,13 @@
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="14">
         <v>7.4219999999999997</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="14">
         <v>7.242</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="14">
         <f t="shared" ref="D20:D25" si="3">ABS(B20)-ABS(C20)</f>
         <v>0.17999999999999972</v>
       </c>
@@ -2365,13 +2436,13 @@
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="14">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="14">
         <f t="shared" si="3"/>
         <v>-1.9E-2</v>
       </c>
@@ -2389,13 +2460,13 @@
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="14">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="14">
         <f t="shared" si="3"/>
         <v>1.0000000000000002E-2</v>
       </c>
@@ -2411,13 +2482,13 @@
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="14">
         <v>-1.4E-2</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="14">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="14">
         <f t="shared" si="3"/>
         <v>-1.1999999999999999E-2</v>
       </c>
@@ -2433,13 +2504,13 @@
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="14">
         <v>-7.2999999999999995E-2</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="14">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="14">
         <f t="shared" si="3"/>
         <v>-1.6E-2</v>
       </c>
@@ -2457,13 +2528,13 @@
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="14">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="14">
         <v>-0.108</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="14">
         <f t="shared" si="3"/>
         <v>-2.8999999999999998E-2</v>
       </c>
@@ -2481,9 +2552,9 @@
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
       <c r="F26" s="1"/>
       <c r="G26" s="4">
         <v>3534.64</v>
@@ -2500,13 +2571,13 @@
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="14">
         <v>7.4210000000000003</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="14">
         <v>7.2229999999999999</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="14">
         <f t="shared" ref="D27:D29" si="4">ABS(B27)-ABS(C27)</f>
         <v>0.1980000000000004</v>
       </c>
@@ -2524,13 +2595,13 @@
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="14">
         <v>-0.222</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="14">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="14">
         <f t="shared" si="4"/>
         <v>-7.5999999999999984E-2</v>
       </c>
@@ -2548,13 +2619,13 @@
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="14">
         <v>0.121</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="14">
         <v>0.153</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="14">
         <f t="shared" si="4"/>
         <v>-3.2000000000000001E-2</v>
       </c>
@@ -2565,16 +2636,14 @@
         <v>26</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="H29" s="4"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
       <c r="F30" s="1"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -2584,13 +2653,16 @@
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
       <c r="F31" s="1"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="1"/>
+      <c r="I31" s="4">
+        <f>AVERAGE(I3:I28)</f>
+        <v>802.50839999999994</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D31">
@@ -2630,542 +2702,1322 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="7" width="18" customWidth="1"/>
+    <col min="8" max="9" width="21.5703125" customWidth="1"/>
+    <col min="10" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="14" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="I1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="22" t="str">
+        <f>CONCATENATE("|",A1,"|",B1,"|",C1,"|",E1,"|",H1,"|",L1,"|")</f>
+        <v>||Original Publication|Reproduce with Author's Data in R|Reanalyze with Local RR in R|Reanalyze with Cluster RR in R|Variance|</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="N2" s="22" t="str">
+        <f t="shared" ref="N2:N28" si="0">CONCATENATE("|",A2,"|",B2,"|",C2,"|",E2,"|",H2,"|",L2,"|")</f>
+        <v>|H2.1 Race Model||||||</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="14">
         <v>7.1059999999999999</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="14">
         <v>6.7809999999999997</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14">
         <v>7.7229999999999999</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14">
         <v>7.37</v>
       </c>
-      <c r="F3" s="14">
-        <f>_xlfn.VAR.P(B3:E3)</f>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14">
+        <f>_xlfn.VAR.P(B3,C3,E3,H3)</f>
         <v>0.11968150000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|(Intercept)|7.106|6.781|7.723|7.37|0.1196815|</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="14">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="14">
         <v>-0.20300000000000001</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="14">
+        <f>ABS(C4-B4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
         <v>-0.129</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F4" s="14">
+        <f>ABS(E4-$B4)</f>
+        <v>7.400000000000001E-2</v>
+      </c>
+      <c r="G4" s="14">
+        <f>ABS(E4-$C4)</f>
+        <v>7.400000000000001E-2</v>
+      </c>
+      <c r="H4" s="14">
         <v>-0.16300000000000001</v>
       </c>
-      <c r="F4" s="14">
-        <f t="shared" ref="F4:F8" si="0">_xlfn.VAR.P(B4:E4)</f>
+      <c r="I4" s="14">
+        <f>ABS(H4-$B4)</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="J4" s="14">
+        <f>ABS(H4-$C4)</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="K4" s="14">
+        <f>ABS(H4-E4)</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" ref="L4:L8" si="1">_xlfn.VAR.P(B4,C4,E4,H4)</f>
         <v>9.5674999999999927E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N4" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|white_pct|-0.203|-0.203|-0.129|-0.163|0.000956749999999999|</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="14">
         <v>0.111</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="14">
         <v>0.33900000000000002</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="14">
+        <f t="shared" ref="D5:D8" si="2">ABS(C5-B5)</f>
+        <v>0.22800000000000004</v>
+      </c>
+      <c r="E5" s="14">
         <v>1.9E-2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="F5" s="14">
+        <f t="shared" ref="F5:I8" si="3">ABS(E5-$B5)</f>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:G8" si="4">ABS(E5-$C5)</f>
+        <v>0.32</v>
+      </c>
+      <c r="H5" s="14">
         <v>0.104</v>
       </c>
-      <c r="F5" s="14">
+      <c r="I5" s="14">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000062E-3</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" ref="J5:J8" si="5">ABS(H5-$C5)</f>
+        <v>0.23500000000000004</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" ref="K5:K8" si="6">ABS(H5-E5)</f>
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="1"/>
+        <v>1.4084187499999998E-2</v>
+      </c>
+      <c r="N5" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1.4084187499999998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>|black_pct|0.111|0.339|0.019|0.104|0.0140841875|</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="14">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="14">
         <v>0.02</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="14">
+        <f t="shared" si="2"/>
+        <v>3.0999999999999996E-2</v>
+      </c>
+      <c r="E6" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F6" s="14">
+        <f t="shared" si="3"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="4"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+      <c r="H6" s="14">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="I6" s="14">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="5"/>
+        <v>1.5999999999999997E-2</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="6"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="1"/>
+        <v>1.7868750000000003E-4</v>
+      </c>
+      <c r="N6" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1.7868750000000003E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>|native_pct|0.051|0.02|0.018|0.036|0.0001786875|</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="14">
         <v>0.08</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="14">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="14">
+        <f t="shared" si="2"/>
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="14">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="3"/>
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="4"/>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="H7" s="14">
         <v>3.9E-2</v>
       </c>
-      <c r="F7" s="14">
+      <c r="I7" s="14">
+        <f t="shared" si="3"/>
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="5"/>
+        <v>1.9000000000000003E-2</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="6"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="1"/>
+        <v>4.6718749999999972E-4</v>
+      </c>
+      <c r="N7" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>4.6718749999999972E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>|asian_pct|0.08|0.058|0.022|0.039|0.0004671875|</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="14">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="14">
         <v>0.108</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="14">
+        <f t="shared" si="2"/>
+        <v>3.1E-2</v>
+      </c>
+      <c r="E8" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="4"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="H8" s="14">
         <v>0.01</v>
       </c>
-      <c r="F8" s="14">
+      <c r="I8" s="14">
+        <f t="shared" si="3"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="5"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="6"/>
+        <v>1.1999999999999999E-2</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="1"/>
+        <v>1.6011874999999989E-3</v>
+      </c>
+      <c r="N8" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1.6011874999999989E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>|other_pct|0.077|0.108|0.022|0.01|0.0016011875|</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="N9" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|H2.2 Ethnicity Model||||||</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="14">
         <v>7.1859999999999999</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="14">
         <v>6.7720000000000002</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14">
         <v>7.7160000000000002</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14">
         <v>7.36</v>
       </c>
-      <c r="F10" s="14">
-        <f t="shared" ref="F10:F28" si="1">_xlfn.VAR.P(B10:E10)</f>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14">
+        <f t="shared" ref="L10:L13" si="7">_xlfn.VAR.P(B10,C10,E10,H10)</f>
         <v>0.11538675</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|(Intercept)|7.186|6.772|7.716|7.36|0.11538675|</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="14">
         <v>-0.23699999999999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="14">
         <v>-0.22800000000000001</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="14">
+        <f t="shared" ref="D11:D13" si="8">ABS(C11-B11)</f>
+        <v>8.9999999999999802E-3</v>
+      </c>
+      <c r="E11" s="14">
         <v>-0.15</v>
       </c>
-      <c r="E11" s="6">
+      <c r="F11" s="14">
+        <f t="shared" ref="F11:I13" si="9">ABS(E11-$B11)</f>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" ref="G11:G13" si="10">ABS(E11-$C11)</f>
+        <v>7.8000000000000014E-2</v>
+      </c>
+      <c r="H11" s="14">
         <v>-0.19</v>
       </c>
-      <c r="F11" s="14">
-        <f t="shared" si="1"/>
+      <c r="I11" s="14">
+        <f t="shared" si="9"/>
+        <v>4.6999999999999986E-2</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" ref="J11:J13" si="11">ABS(H11-$C11)</f>
+        <v>3.8000000000000006E-2</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" ref="K11:K13" si="12">ABS(H11-E11)</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="7"/>
         <v>1.1866875000000054E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N11" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|non_hisp_white_pct|-0.237|-0.228|-0.15|-0.19|0.00118668750000001|</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="14">
         <v>0.11899999999999999</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="14">
         <v>0.13200000000000001</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="14">
+        <f t="shared" si="8"/>
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="E12" s="14">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E12" s="6">
+      <c r="F12" s="14">
+        <f t="shared" si="9"/>
+        <v>0.11299999999999999</v>
+      </c>
+      <c r="G12" s="14">
+        <f t="shared" si="10"/>
+        <v>0.126</v>
+      </c>
+      <c r="H12" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="14">
-        <f t="shared" si="1"/>
+      <c r="I12" s="14">
+        <f t="shared" si="9"/>
+        <v>0.11399999999999999</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" si="11"/>
+        <v>0.127</v>
+      </c>
+      <c r="K12" s="14">
+        <f t="shared" si="12"/>
+        <v>1E-3</v>
+      </c>
+      <c r="L12" s="14">
+        <f t="shared" si="7"/>
         <v>3.6212499999999995E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N12" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|hisp_pct|0.119|0.132|0.006|0.005|0.00362125|</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="14">
         <v>0.11799999999999999</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="14">
         <v>0.33500000000000002</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="14">
+        <f t="shared" si="8"/>
+        <v>0.21700000000000003</v>
+      </c>
+      <c r="E13" s="14">
         <v>2.3E-2</v>
       </c>
-      <c r="E13" s="6">
+      <c r="F13" s="14">
+        <f t="shared" si="9"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G13" s="14">
+        <f t="shared" si="10"/>
+        <v>0.312</v>
+      </c>
+      <c r="H13" s="14">
         <v>0.105</v>
       </c>
-      <c r="F13" s="14">
-        <f t="shared" si="1"/>
+      <c r="I13" s="14">
+        <f t="shared" si="9"/>
+        <v>1.2999999999999998E-2</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" si="11"/>
+        <v>0.23000000000000004</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="12"/>
+        <v>8.199999999999999E-2</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="7"/>
         <v>1.3328187499999998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N13" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|non_hisp_non_white_pct|0.118|0.335|0.023|0.105|0.0133281875|</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="N14" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|H2.3 Poverty Model||||||</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="14">
         <v>7.1829999999999998</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="14">
         <v>6.8490000000000002</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14">
         <v>7.774</v>
       </c>
-      <c r="E15" s="6">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14">
         <v>7.3819999999999997</v>
       </c>
-      <c r="F15" s="14">
-        <f t="shared" si="1"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14">
+        <f t="shared" ref="L15:L17" si="13">_xlfn.VAR.P(B15,C15,E15,H15)</f>
         <v>0.11211349999999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N15" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|(Intercept)|7.183|6.849|7.774|7.382|0.1121135|</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="14">
         <v>0.14799999999999999</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="14">
         <v>0.28299999999999997</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="14">
+        <f t="shared" ref="D16:D17" si="14">ABS(C16-B16)</f>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="E16" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E16" s="6">
+      <c r="F16" s="14">
+        <f t="shared" ref="F16:I17" si="15">ABS(E16-$B16)</f>
+        <v>0.13</v>
+      </c>
+      <c r="G16" s="14">
+        <f>ABS(E16-$C16)</f>
+        <v>0.26499999999999996</v>
+      </c>
+      <c r="H16" s="14">
         <v>0.109</v>
       </c>
-      <c r="F16" s="14">
-        <f t="shared" si="1"/>
+      <c r="I16" s="14">
+        <f t="shared" si="15"/>
+        <v>3.8999999999999993E-2</v>
+      </c>
+      <c r="J16" s="14">
+        <f>ABS(H16-$C16)</f>
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" ref="K16:K17" si="16">ABS(H16-E16)</f>
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="13"/>
         <v>9.0892500000000001E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N16" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|bpov_pct|0.148|0.283|0.018|0.109|0.00908925|</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="14">
         <v>-0.26700000000000002</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="14">
         <v>-0.315</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="14">
+        <f t="shared" si="14"/>
+        <v>4.7999999999999987E-2</v>
+      </c>
+      <c r="E17" s="14">
         <v>-0.11</v>
       </c>
-      <c r="E17" s="6">
+      <c r="F17" s="14">
+        <f t="shared" si="15"/>
+        <v>0.15700000000000003</v>
+      </c>
+      <c r="G17" s="14">
+        <f>ABS(E17-$C17)</f>
+        <v>0.20500000000000002</v>
+      </c>
+      <c r="H17" s="14">
         <v>-0.19400000000000001</v>
       </c>
-      <c r="F17" s="14">
-        <f t="shared" si="1"/>
+      <c r="I17" s="14">
+        <f t="shared" si="15"/>
+        <v>7.3000000000000009E-2</v>
+      </c>
+      <c r="J17" s="14">
+        <f>ABS(H17-$C17)</f>
+        <v>0.121</v>
+      </c>
+      <c r="K17" s="14">
+        <f t="shared" si="16"/>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" si="13"/>
         <v>6.0002499999999848E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N17" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|apov_pct|-0.267|-0.315|-0.11|-0.194|0.00600024999999998|</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="N18" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|H2.4 Age Model||||||</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="14">
         <v>7.242</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="14">
         <v>6.8639999999999999</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14">
         <v>7.7830000000000004</v>
       </c>
-      <c r="E19" s="6">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14">
         <v>7.4219999999999997</v>
       </c>
-      <c r="F19" s="14">
-        <f t="shared" si="1"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14">
+        <f t="shared" ref="L19:L24" si="17">_xlfn.VAR.P(B19,C19,E19,H19)</f>
         <v>0.10963818750000009</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N19" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|(Intercept)|7.242|6.864|7.783|7.422|0.1096381875|</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="14">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="14">
+        <f t="shared" ref="D20:D24" si="18">ABS(C20-B20)</f>
+        <v>0.03</v>
+      </c>
+      <c r="E20" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E20" s="6">
+      <c r="F20" s="14">
+        <f t="shared" ref="F20:I24" si="19">ABS(E20-$B20)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G20" s="14">
+        <f t="shared" ref="G20:G24" si="20">ABS(E20-$C20)</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="H20" s="14">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F20" s="14">
-        <f t="shared" si="1"/>
+      <c r="I20" s="14">
+        <f t="shared" si="19"/>
+        <v>1.9E-2</v>
+      </c>
+      <c r="J20" s="14">
+        <f t="shared" ref="J20:J24" si="21">ABS(H20-$C20)</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K20" s="14">
+        <f t="shared" ref="K20:K24" si="22">ABS(H20-E20)</f>
+        <v>6.0000000000000019E-3</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" si="17"/>
         <v>4.5925000000000002E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N20" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|pct_5_17|0.047|0.077|0.022|0.028|0.00045925|</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="14">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="14">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="14">
+        <f t="shared" si="18"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="E21" s="14">
         <v>1.4E-2</v>
       </c>
-      <c r="E21" s="6">
+      <c r="F21" s="14">
+        <f t="shared" si="19"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="G21" s="14">
+        <f t="shared" si="20"/>
+        <v>1.1999999999999999E-2</v>
+      </c>
+      <c r="H21" s="14">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F21" s="14">
-        <f t="shared" si="1"/>
+      <c r="I21" s="14">
+        <f t="shared" si="19"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="21"/>
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="22"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L21" s="14">
+        <f t="shared" si="17"/>
         <v>1.6274999999999992E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N21" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|pct_18_34|0.038|0.026|0.014|0.048|0.00016275|</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="14">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="14">
         <v>0.04</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="14">
+        <f t="shared" si="18"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E22" s="14">
         <v>-2.4E-2</v>
       </c>
-      <c r="E22" s="6">
+      <c r="F22" s="14">
+        <f t="shared" si="19"/>
+        <v>1.9999999999999983E-3</v>
+      </c>
+      <c r="G22" s="14">
+        <f t="shared" si="20"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H22" s="14">
         <v>-1.4E-2</v>
       </c>
-      <c r="F22" s="14">
-        <f t="shared" si="1"/>
+      <c r="I22" s="14">
+        <f t="shared" si="19"/>
+        <v>1.1999999999999999E-2</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="21"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K22" s="14">
+        <f t="shared" si="22"/>
+        <v>0.01</v>
+      </c>
+      <c r="L22" s="14">
+        <f t="shared" si="17"/>
         <v>7.2600000000000008E-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N22" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|pct_35_64|-0.026|0.04|-0.024|-0.014|0.000726|</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="14">
         <v>-8.8999999999999996E-2</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="14">
         <v>-2.4E-2</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="14">
+        <f t="shared" si="18"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E23" s="14">
         <v>-5.6000000000000001E-2</v>
       </c>
-      <c r="E23" s="6">
+      <c r="F23" s="14">
+        <f t="shared" si="19"/>
+        <v>3.2999999999999995E-2</v>
+      </c>
+      <c r="G23" s="14">
+        <f t="shared" si="20"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H23" s="14">
         <v>-7.2999999999999995E-2</v>
       </c>
-      <c r="F23" s="14">
-        <f t="shared" si="1"/>
+      <c r="I23" s="14">
+        <f t="shared" si="19"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="J23" s="14">
+        <f t="shared" si="21"/>
+        <v>4.8999999999999995E-2</v>
+      </c>
+      <c r="K23" s="14">
+        <f t="shared" si="22"/>
+        <v>1.6999999999999994E-2</v>
+      </c>
+      <c r="L23" s="14">
+        <f t="shared" si="17"/>
         <v>5.802499999999996E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N23" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|pct_65_74|-0.089|-0.024|-0.056|-0.073|0.00058025|</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="14">
         <v>-0.108</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="14">
         <v>-0.2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="14">
+        <f t="shared" si="18"/>
+        <v>9.2000000000000012E-2</v>
+      </c>
+      <c r="E24" s="14">
         <v>-5.2999999999999999E-2</v>
       </c>
-      <c r="E24" s="6">
+      <c r="F24" s="14">
+        <f t="shared" si="19"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="G24" s="14">
+        <f t="shared" si="20"/>
+        <v>0.14700000000000002</v>
+      </c>
+      <c r="H24" s="14">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="F24" s="14">
-        <f t="shared" si="1"/>
+      <c r="I24" s="14">
+        <f t="shared" si="19"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+      <c r="J24" s="14">
+        <f t="shared" si="21"/>
+        <v>0.12100000000000001</v>
+      </c>
+      <c r="K24" s="14">
+        <f t="shared" si="22"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="L24" s="14">
+        <f t="shared" si="17"/>
         <v>3.0785000000000014E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N24" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|pct_75|-0.108|-0.2|-0.053|-0.079|0.0030785|</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="N25" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|H2.5 Biological Sex Model||||||</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="14">
         <v>7.2229999999999999</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="14">
         <v>6.85</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14">
         <v>7.7839999999999998</v>
       </c>
-      <c r="E26" s="6">
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14">
         <v>7.4210000000000003</v>
       </c>
-      <c r="F26" s="14">
-        <f t="shared" si="1"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14">
+        <f t="shared" ref="L26:L28" si="23">_xlfn.VAR.P(B26,C26,E26,H26)</f>
         <v>0.11395125000000006</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N26" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|(Intercept)|7.223|6.85|7.784|7.421|0.11395125|</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="14">
         <v>-0.29799999999999999</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="14">
         <v>-0.46700000000000003</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="14">
+        <f t="shared" ref="D27:D28" si="24">ABS(C27-B27)</f>
+        <v>0.16900000000000004</v>
+      </c>
+      <c r="E27" s="14">
         <v>-0.13500000000000001</v>
       </c>
-      <c r="E27" s="6">
+      <c r="F27" s="14">
+        <f t="shared" ref="F27:I28" si="25">ABS(E27-$B27)</f>
+        <v>0.16299999999999998</v>
+      </c>
+      <c r="G27" s="14">
+        <f t="shared" ref="G27:G28" si="26">ABS(E27-$C27)</f>
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="H27" s="14">
         <v>-0.222</v>
       </c>
-      <c r="F27" s="14">
-        <f t="shared" si="1"/>
+      <c r="I27" s="14">
+        <f t="shared" si="25"/>
+        <v>7.5999999999999984E-2</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" ref="J27:J28" si="27">ABS(H27-$C27)</f>
+        <v>0.24500000000000002</v>
+      </c>
+      <c r="K27" s="14">
+        <f t="shared" ref="K27:K28" si="28">ABS(H27-E27)</f>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" si="23"/>
         <v>1.4920249999999982E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="N27" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|male_pct|-0.298|-0.467|-0.135|-0.222|0.01492025|</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="14">
         <v>0.153</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="14">
         <v>0.38</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="14">
+        <f t="shared" si="24"/>
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E28" s="14">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="E28" s="6">
+      <c r="F28" s="14">
+        <f t="shared" si="25"/>
+        <v>0.11199999999999999</v>
+      </c>
+      <c r="G28" s="14">
+        <f t="shared" si="26"/>
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="H28" s="14">
         <v>0.121</v>
       </c>
-      <c r="F28" s="14">
+      <c r="I28" s="14">
+        <f t="shared" si="25"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="J28" s="14">
+        <f t="shared" si="27"/>
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="K28" s="14">
+        <f t="shared" si="28"/>
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="L28" s="14">
+        <f t="shared" si="23"/>
+        <v>1.5843687499999985E-2</v>
+      </c>
+      <c r="N28" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>|female_pct|0.153|0.38|0.041|0.121|0.0158436875|</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18">
+        <f>AVERAGE(D4:D28)</f>
+        <v>8.2058823529411781E-2</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="18">
+        <f>AVERAGE(F4:F28)</f>
+        <v>7.6941176470588249E-2</v>
+      </c>
+      <c r="G30" s="18">
+        <f>AVERAGE(G4:G28)</f>
+        <v>0.1461764705882353</v>
+      </c>
+      <c r="H30" s="19"/>
+      <c r="I30" s="18">
+        <f>AVERAGE(I4:I28)</f>
+        <v>3.8235294117647062E-2</v>
+      </c>
+      <c r="J30" s="18">
+        <f>AVERAGE(J4:J28)</f>
+        <v>0.11158823529411765</v>
+      </c>
+      <c r="K30" s="18">
+        <f>AVERAGE(K4:K28)</f>
+        <v>4.2588235294117649E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I1:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" style="10" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="str">
+        <f>CONCATENATE("|",A1)</f>
+        <v>|</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE(F1,"|",B1)</f>
+        <v>||Original Study</v>
+      </c>
+      <c r="H1" t="str">
+        <f t="shared" ref="H1:I1" si="0">CONCATENATE(G1,"|",C1)</f>
+        <v>||Original Study|Original Data in R/geepack</v>
+      </c>
+      <c r="I1" t="str">
+        <f>CONCATENATE(H1,"|",D1,"|")</f>
+        <v>||Original Study|Original Data in R/geepack|Reproduced local relative risk|</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="F2" t="str">
+        <f>CONCATENATE("|",A2)</f>
+        <v>|Original Data in R/geepack</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:I2" si="1">CONCATENATE(F2,"|",B2)</f>
+        <v>|Original Data in R/geepack|0.082</v>
+      </c>
+      <c r="H2" t="str">
         <f t="shared" si="1"/>
-        <v>1.5843687499999985E-2</v>
+        <v>|Original Data in R/geepack|0.082|</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I4" si="2">CONCATENATE(H2,"|",D2,"|")</f>
+        <v>|Original Data in R/geepack|0.082|||</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="21">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F4" si="3">CONCATENATE("|",A3)</f>
+        <v>|Reproduced local relative risk</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:I3" si="4">CONCATENATE(F3,"|",B3)</f>
+        <v>|Reproduced local relative risk|0.077</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="4"/>
+        <v>|Reproduced local relative risk|0.077|0.146</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="2"/>
+        <v>|Reproduced local relative risk|0.077|0.146||</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="20">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0.122</v>
+      </c>
+      <c r="D4" s="20">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>|Reproduced cluster relative risk</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:I4" si="5">CONCATENATE(F4,"|",B4)</f>
+        <v>|Reproduced cluster relative risk|0.038</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="5"/>
+        <v>|Reproduced cluster relative risk|0.038|0.122</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>|Reproduced cluster relative risk|0.038|0.122|0.043|</v>
       </c>
     </row>
   </sheetData>

</xml_diff>